<commit_message>
Fixed mu problem and also added info about weight of reference individual in age and gender group for the EAR protein calculation.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/DRI_IOM_V4.xlsx
+++ b/data-raw/NutrientData/DRI_IOM_V4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="2060" windowWidth="24080" windowHeight="14600" activeTab="1"/>
+    <workbookView xWindow="1520" yWindow="2060" windowWidth="24080" windowHeight="14600" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="10" r:id="rId1"/>
@@ -937,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2570,7 +2570,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="12" width="8.83203125" style="1"/>
+    <col min="1" max="3" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="12" width="8.83203125" style="1"/>
     <col min="13" max="13" width="10.5" style="1" customWidth="1"/>
     <col min="14" max="16384" width="8.83203125" style="1"/>
   </cols>
@@ -3805,7 +3807,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5128,7 +5130,8 @@
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
     <col min="6" max="7" width="8.83203125" style="1"/>
     <col min="8" max="8" width="12.1640625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="1"/>
+    <col min="9" max="9" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="17" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -7608,8 +7611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:T1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="D1:T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>